<commit_message>
Updated bead voltages file with new values and changed name to correct the fact that there are voltages for multiple instruments within the one file
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cheese\Instrument_Logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\from_Samwise\ifcb-analysis\IFCB_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="IFCB101" sheetId="4" r:id="rId4"/>
     <sheet name="IFCB102" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="179">
   <si>
     <t>File D</t>
   </si>
@@ -500,6 +500,78 @@
   </si>
   <si>
     <t>0.1-0.16</t>
+  </si>
+  <si>
+    <t>hv(chl)</t>
+  </si>
+  <si>
+    <t>IFCB1_2015_124_102422</t>
+  </si>
+  <si>
+    <t>1.8-2.7</t>
+  </si>
+  <si>
+    <t>0.3-0.55</t>
+  </si>
+  <si>
+    <t>beads in the field</t>
+  </si>
+  <si>
+    <t>high %missed roi because small cells in water?</t>
+  </si>
+  <si>
+    <t>select signals</t>
+  </si>
+  <si>
+    <t>39% missed in this file</t>
+  </si>
+  <si>
+    <t>IFCB1_2015_121_225419</t>
+  </si>
+  <si>
+    <t>1.7-2.8</t>
+  </si>
+  <si>
+    <t>0.2-0.5</t>
+  </si>
+  <si>
+    <t>20% missed in this file</t>
+  </si>
+  <si>
+    <t>IFCB5_2015_264_162243</t>
+  </si>
+  <si>
+    <t>-1.413 - -1.435</t>
+  </si>
+  <si>
+    <t>0.7-1.7</t>
+  </si>
+  <si>
+    <t>9um beads in FSW in lab, new comp stack and new cytopia board, something off in board? PMTs misaligned?</t>
+  </si>
+  <si>
+    <t>IFCB5_2014_258_220252</t>
+  </si>
+  <si>
+    <t>last beads fun at MVCO before recovery</t>
+  </si>
+  <si>
+    <t>1.4-1.7</t>
+  </si>
+  <si>
+    <t>1-1.7</t>
+  </si>
+  <si>
+    <t>IFCB5_2015_275_180649</t>
+  </si>
+  <si>
+    <t>1.8-2.3</t>
+  </si>
+  <si>
+    <t>9um beads in FSW in lab, 'new' board after Alexi fixed solder on R12</t>
+  </si>
+  <si>
+    <t>hvA(chl)</t>
   </si>
 </sst>
 </file>
@@ -541,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,6 +639,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,13 +1428,13 @@
     <col min="9" max="9" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="2"/>
     <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1371,40 +1445,44 @@
         <v>33</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -1414,44 +1492,44 @@
       <c r="C2" s="3">
         <v>191851</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>2</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>6.5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>19.2</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>0.35</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>6.5</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>19.2</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -1461,41 +1539,41 @@
       <c r="C3" s="3">
         <v>193104</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>7.2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>9.5</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>0.38</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>18.8</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>33.4</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1505,41 +1583,41 @@
       <c r="C4" s="3">
         <v>165315</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>10.9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>25.6</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>0.61</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>40.9</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>45.1</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -1549,41 +1627,41 @@
       <c r="C5" s="3">
         <v>191634</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>9</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>0.62</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>41.2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>30</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -1593,41 +1671,42 @@
       <c r="C6" s="3">
         <v>203331</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>10.199999999999999</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>27.4</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>0.61</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>41.3</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>47.5</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1637,47 +1716,47 @@
       <c r="C7" s="3">
         <v>165104</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>11.1</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>27.5</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>43.8</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>43.5</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -1687,47 +1766,47 @@
       <c r="C8" s="3">
         <v>182317</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>2.1</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>8.6</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>22.4</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>0.32</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>14.8</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>35</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1737,44 +1816,44 @@
       <c r="C9" s="3">
         <v>191226</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>7.9</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>20.9</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>0.27</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>35.5</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>62.9</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="P9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -1784,38 +1863,39 @@
       <c r="C10" s="3">
         <v>191226</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>8.5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>14.9</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>0.32</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>42.5</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>59.1</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="3"/>
+      <c r="N10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -1825,32 +1905,34 @@
       <c r="C11" s="3">
         <v>163302</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>10.199999999999999</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>30.1</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>0.35</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>29.6</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>76.3</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>76</v>
       </c>
@@ -1860,75 +1942,183 @@
       <c r="C12" s="3">
         <v>171644</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>11</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>29.9</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>0.33</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>41.9</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>105.4</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3"/>
+      <c r="N12" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="6">
+        <v>42125</v>
+      </c>
+      <c r="C13" s="3">
+        <v>225419</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G13" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="H13" s="3">
+        <v>13.8</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="K13" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="L13" s="3">
+        <v>41.2</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="6">
+        <v>42128</v>
+      </c>
+      <c r="C14" s="3">
+        <v>102422</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G14" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>12.3</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.38</v>
+      </c>
+      <c r="K14" s="3">
+        <v>19</v>
+      </c>
+      <c r="L14" s="3">
+        <v>34.6</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B15" s="6">
         <v>42158</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C15" s="3">
         <v>83918</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F15" s="3">
         <v>2</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G15" s="3">
         <v>8.6</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H15" s="3">
         <v>13.4</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J15" s="3">
         <v>0.3</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K15" s="3">
         <v>27.7</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L15" s="3">
         <v>63.2</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1940,23 +2130,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1967,83 +2157,214 @@
         <v>33</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="8">
+        <v>41897</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.91805555555555562</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>1.4</v>
+      </c>
+      <c r="G2">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="H2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="J2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2">
+        <v>1.2</v>
+      </c>
+      <c r="L2">
+        <v>22.2</v>
+      </c>
+      <c r="M2">
+        <v>22.5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B3" s="8">
         <v>42033</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C3" s="9">
         <v>0.95000000000000007</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E2">
+      <c r="F3">
         <v>1.5</v>
       </c>
-      <c r="F2">
+      <c r="G3">
         <v>17.2</v>
       </c>
-      <c r="G2">
+      <c r="H3">
         <v>12.4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J3" t="s">
         <v>92</v>
       </c>
-      <c r="I2">
+      <c r="K3">
         <v>1.6</v>
       </c>
-      <c r="J2">
+      <c r="L3">
         <v>21.4</v>
       </c>
-      <c r="K2">
+      <c r="M3">
         <v>15.2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N3" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O3" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="8">
+        <v>42264</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>-1.5</v>
+      </c>
+      <c r="G4">
+        <v>-2.4</v>
+      </c>
+      <c r="H4">
+        <v>36.5</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="K4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L4">
+        <v>66.7</v>
+      </c>
+      <c r="M4">
+        <v>44.1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>169</v>
+      </c>
+      <c r="O4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="8">
+        <v>42279</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.75416666666666676</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="F5">
+        <v>1.7</v>
+      </c>
+      <c r="G5">
+        <v>55.4</v>
+      </c>
+      <c r="H5">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="J5" t="s">
+        <v>176</v>
+      </c>
+      <c r="K5">
+        <v>1.2</v>
+      </c>
+      <c r="L5">
+        <v>65.5</v>
+      </c>
+      <c r="M5">
+        <v>44.5</v>
+      </c>
+      <c r="N5" s="12">
+        <v>42006</v>
+      </c>
+      <c r="O5" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2051,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2445,7 +2766,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Taylor updated bead voltage entries
</commit_message>
<xml_diff>
--- a/IFCB_tools/IFCB_beadvoltages.xlsx
+++ b/IFCB_tools/IFCB_beadvoltages.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cheese\Instrument_Logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ifcb-analysis\IFCB_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="15015" windowHeight="1290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IFCB10" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="157">
   <si>
     <t>File D</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>0.1-0.16</t>
+  </si>
+  <si>
+    <t>IFCB5_2015_285_180748</t>
+  </si>
+  <si>
+    <t>9um beads in SW after changing delay to about 270us guess that's not what it was before. Could be new board?</t>
   </si>
 </sst>
 </file>
@@ -1940,10 +1946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,6 +2048,38 @@
         <v>90</v>
       </c>
     </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="8">
+        <v>42289</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="E3">
+        <v>1.6</v>
+      </c>
+      <c r="F3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G3">
+        <v>7.7</v>
+      </c>
+      <c r="I3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J3">
+        <v>24.8</v>
+      </c>
+      <c r="K3">
+        <v>41.5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2051,7 +2089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>